<commit_message>
Version 1 is done for lab 1 version 2 is 75% of the way done for both programs. Study hours were updated on the hours sheet.
</commit_message>
<xml_diff>
--- a/ClassHours.xlsx
+++ b/ClassHours.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21126"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1DFDBC02-D941-4046-B855-01241B41593C}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{99FD3B25-8471-43AD-A28D-C7FB2607FA2F}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
   <si>
     <t>Hours Worked</t>
   </si>
@@ -71,6 +71,9 @@
   </si>
   <si>
     <t>TicTacToe and Stopwatch with the group</t>
+  </si>
+  <si>
+    <t>Worked on V2 of TTT and Stopwatch. Finished more of the quizzes. 1 hour on Monday 4 on Thursday 2 on Sunday</t>
   </si>
 </sst>
 </file>
@@ -391,7 +394,7 @@
   <dimension ref="A1:D11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E1" sqref="E1"/>
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -399,7 +402,7 @@
     <col min="1" max="1" width="15.6640625" customWidth="1"/>
     <col min="2" max="2" width="18.6640625" customWidth="1"/>
     <col min="3" max="3" width="17.21875" customWidth="1"/>
-    <col min="4" max="4" width="34.5546875" customWidth="1"/>
+    <col min="4" max="4" width="80.21875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.3">
@@ -443,8 +446,17 @@
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A4">
+        <v>7</v>
+      </c>
       <c r="B4" t="s">
         <v>5</v>
+      </c>
+      <c r="C4">
+        <v>48</v>
+      </c>
+      <c r="D4" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
update notes in spreadsheet
</commit_message>
<xml_diff>
--- a/ClassHours.xlsx
+++ b/ClassHours.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21126"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{99FD3B25-8471-43AD-A28D-C7FB2607FA2F}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0A15198C-0F77-45B6-8A5D-42AAAF32A088}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
   <si>
     <t>Hours Worked</t>
   </si>
@@ -74,6 +74,9 @@
   </si>
   <si>
     <t>Worked on V2 of TTT and Stopwatch. Finished more of the quizzes. 1 hour on Monday 4 on Thursday 2 on Sunday</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Worked on the TODO list and got it finsihed. Going to start on the Bookmark lab. Gonna work on that tomorrow. </t>
   </si>
 </sst>
 </file>
@@ -394,7 +397,7 @@
   <dimension ref="A1:D11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -460,8 +463,17 @@
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A5">
+        <v>4</v>
+      </c>
       <c r="B5" t="s">
         <v>6</v>
+      </c>
+      <c r="C5">
+        <v>44</v>
+      </c>
+      <c r="D5" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.3">

</xml_diff>